<commit_message>
Downloaded CSVs are now moved to the character_data/ folder, instead of seperate folders.
</commit_message>
<xml_diff>
--- a/warcraftLogs/character_data/character_data.xlsx
+++ b/warcraftLogs/character_data/character_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matth\git\DataAnalysisWorkbooks\warcraftLogs\character_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D314C1A3-9AD3-4E96-A348-F88591FF2751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E08A92-7867-4190-B0BB-CB84CF5322D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1103" yWindow="1103" windowWidth="13590" windowHeight="7822" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -713,6 +713,27 @@
     <t xml:space="preserve"> ['2LB 2I'</t>
   </si>
   <si>
+    <t>Mar 5 2022</t>
+  </si>
+  <si>
+    <t>1:12</t>
+  </si>
+  <si>
+    <t>1069.3</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.333]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ['2LB 1I 1RG'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.154]]"</t>
+  </si>
+  <si>
     <t>1:17</t>
   </si>
   <si>
@@ -722,13 +743,7 @@
     <t>0.69</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.333]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ['2LB 1I 1RG'</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.154]]"</t>
+    <t xml:space="preserve"> 0.133]]"</t>
   </si>
   <si>
     <t>1:24</t>
@@ -752,7 +767,7 @@
     <t>"[['1LB 1I'</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.133]]"</t>
+    <t xml:space="preserve"> ['Other'</t>
   </si>
   <si>
     <t>1:10</t>
@@ -773,7 +788,7 @@
     <t xml:space="preserve"> 0.385]</t>
   </si>
   <si>
-    <t xml:space="preserve"> ['Other'</t>
+    <t xml:space="preserve"> 0.231]]"</t>
   </si>
   <si>
     <t>1:13</t>
@@ -791,9 +806,6 @@
     <t xml:space="preserve"> 0.462]</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.231]]"</t>
-  </si>
-  <si>
     <t>41</t>
   </si>
   <si>
@@ -818,18 +830,6 @@
     <t>502.5</t>
   </si>
   <si>
-    <t>Mar 5 2022</t>
-  </si>
-  <si>
-    <t>1:12</t>
-  </si>
-  <si>
-    <t>1069.3</t>
-  </si>
-  <si>
-    <t>0.77</t>
-  </si>
-  <si>
     <t>2:22</t>
   </si>
   <si>
@@ -1631,6 +1631,51 @@
     <t>802.5</t>
   </si>
   <si>
+    <t>2:07</t>
+  </si>
+  <si>
+    <t>97.52%</t>
+  </si>
+  <si>
+    <t>744.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.188]]"</t>
+  </si>
+  <si>
+    <t>1:59</t>
+  </si>
+  <si>
+    <t>719.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.5]</t>
+  </si>
+  <si>
+    <t>99.44%</t>
+  </si>
+  <si>
+    <t>630.0</t>
+  </si>
+  <si>
+    <t>1:36</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>423.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.294]]"</t>
+  </si>
+  <si>
+    <t>98.51%</t>
+  </si>
+  <si>
+    <t>471.5</t>
+  </si>
+  <si>
     <t>1:52</t>
   </si>
   <si>
@@ -1640,70 +1685,25 @@
     <t>682.9</t>
   </si>
   <si>
-    <t xml:space="preserve"> 0.5]</t>
+    <t>1071.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.316]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.263]]"</t>
+  </si>
+  <si>
+    <t>1:45</t>
+  </si>
+  <si>
+    <t>1009.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.353]</t>
   </si>
   <si>
     <t xml:space="preserve"> 0.235]]"</t>
-  </si>
-  <si>
-    <t>2:07</t>
-  </si>
-  <si>
-    <t>97.52%</t>
-  </si>
-  <si>
-    <t>744.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.188]]"</t>
-  </si>
-  <si>
-    <t>1:59</t>
-  </si>
-  <si>
-    <t>719.4</t>
-  </si>
-  <si>
-    <t>99.44%</t>
-  </si>
-  <si>
-    <t>630.0</t>
-  </si>
-  <si>
-    <t>1:36</t>
-  </si>
-  <si>
-    <t>36</t>
-  </si>
-  <si>
-    <t>423.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.294]]"</t>
-  </si>
-  <si>
-    <t>98.51%</t>
-  </si>
-  <si>
-    <t>471.5</t>
-  </si>
-  <si>
-    <t>1071.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.316]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.263]]"</t>
-  </si>
-  <si>
-    <t>1:45</t>
-  </si>
-  <si>
-    <t>1009.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0.353]</t>
   </si>
   <si>
     <t>1:47</t>
@@ -3066,7 +3066,7 @@
   <dimension ref="A1:S10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3168,7 +3168,7 @@
         <v>30</v>
       </c>
       <c r="P2" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="Q2" t="s">
         <v>159</v>
@@ -3289,7 +3289,7 @@
         <v>142</v>
       </c>
       <c r="Q4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R4" t="s">
         <v>33</v>
@@ -3309,13 +3309,13 @@
         <v>221</v>
       </c>
       <c r="D5" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="E5" t="s">
         <v>205</v>
       </c>
       <c r="F5" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="G5" t="s">
         <v>22</v>
@@ -3327,7 +3327,7 @@
         <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>534</v>
+        <v>549</v>
       </c>
       <c r="K5" t="s">
         <v>114</v>
@@ -3348,13 +3348,13 @@
         <v>31</v>
       </c>
       <c r="Q5" t="s">
+        <v>538</v>
+      </c>
+      <c r="R5" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" t="s">
         <v>535</v>
-      </c>
-      <c r="R5" t="s">
-        <v>80</v>
-      </c>
-      <c r="S5" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -3368,7 +3368,7 @@
         <v>48</v>
       </c>
       <c r="D6" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E6" t="s">
         <v>37</v>
@@ -3383,10 +3383,10 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="J6" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="K6" t="s">
         <v>29</v>
@@ -3398,7 +3398,7 @@
         <v>116</v>
       </c>
       <c r="N6" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="O6" t="s">
         <v>42</v>
@@ -3410,10 +3410,10 @@
         <v>117</v>
       </c>
       <c r="R6" t="s">
-        <v>70</v>
+        <v>154</v>
       </c>
       <c r="S6" t="s">
-        <v>540</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.45">
@@ -3427,7 +3427,7 @@
         <v>338</v>
       </c>
       <c r="D7" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="E7" t="s">
         <v>37</v>
@@ -3445,7 +3445,7 @@
         <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="K7" t="s">
         <v>150</v>
@@ -3466,13 +3466,13 @@
         <v>31</v>
       </c>
       <c r="Q7" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="R7" t="s">
         <v>154</v>
       </c>
       <c r="S7" t="s">
-        <v>216</v>
+        <v>398</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -3501,10 +3501,10 @@
         <v>23</v>
       </c>
       <c r="I8" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="J8" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="K8" t="s">
         <v>114</v>
@@ -3528,10 +3528,10 @@
         <v>452</v>
       </c>
       <c r="R8" t="s">
-        <v>154</v>
+        <v>33</v>
       </c>
       <c r="S8" t="s">
-        <v>398</v>
+        <v>544</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -3545,10 +3545,10 @@
         <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="E9" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -3563,7 +3563,7 @@
         <v>198</v>
       </c>
       <c r="J9" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="K9" t="s">
         <v>295</v>
@@ -3584,13 +3584,13 @@
         <v>142</v>
       </c>
       <c r="Q9" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="R9" t="s">
         <v>33</v>
       </c>
       <c r="S9" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -3619,13 +3619,13 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="J10" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="K10" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="L10" t="s">
         <v>134</v>
@@ -3649,10 +3649,13 @@
         <v>33</v>
       </c>
       <c r="S10" t="s">
-        <v>548</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q10">
+    <sortCondition descending="1" ref="E1"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -3726,7 +3729,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -3744,7 +3747,7 @@
         <v>52</v>
       </c>
       <c r="J2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="K2" t="s">
         <v>295</v>
@@ -3765,13 +3768,13 @@
         <v>428</v>
       </c>
       <c r="Q2" t="s">
+        <v>551</v>
+      </c>
+      <c r="R2" t="s">
+        <v>231</v>
+      </c>
+      <c r="S2" t="s">
         <v>552</v>
-      </c>
-      <c r="R2" t="s">
-        <v>230</v>
-      </c>
-      <c r="S2" t="s">
-        <v>553</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.45">
@@ -3785,7 +3788,7 @@
         <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="E3" t="s">
         <v>205</v>
@@ -3803,7 +3806,7 @@
         <v>52</v>
       </c>
       <c r="J3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K3" t="s">
         <v>140</v>
@@ -3824,13 +3827,13 @@
         <v>428</v>
       </c>
       <c r="Q3" t="s">
+        <v>555</v>
+      </c>
+      <c r="R3" t="s">
+        <v>231</v>
+      </c>
+      <c r="S3" t="s">
         <v>556</v>
-      </c>
-      <c r="R3" t="s">
-        <v>230</v>
-      </c>
-      <c r="S3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -4080,7 +4083,7 @@
         <v>61</v>
       </c>
       <c r="D8" t="s">
-        <v>532</v>
+        <v>547</v>
       </c>
       <c r="E8" t="s">
         <v>395</v>
@@ -4122,7 +4125,7 @@
         <v>188</v>
       </c>
       <c r="R8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S8" t="s">
         <v>398</v>
@@ -4178,7 +4181,7 @@
         <v>31</v>
       </c>
       <c r="Q9" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R9" t="s">
         <v>225</v>
@@ -4379,7 +4382,7 @@
         <v>83</v>
       </c>
       <c r="D3" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -4400,7 +4403,7 @@
         <v>582</v>
       </c>
       <c r="K3" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
@@ -4536,7 +4539,7 @@
         <v>45</v>
       </c>
       <c r="Q5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R5" t="s">
         <v>70</v>
@@ -4577,7 +4580,7 @@
         <v>592</v>
       </c>
       <c r="K6" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="L6" t="s">
         <v>151</v>
@@ -4595,7 +4598,7 @@
         <v>45</v>
       </c>
       <c r="Q6" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="R6" t="s">
         <v>154</v>
@@ -4660,7 +4663,7 @@
         <v>33</v>
       </c>
       <c r="S7" t="s">
-        <v>536</v>
+        <v>556</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -4897,7 +4900,7 @@
         <v>608</v>
       </c>
       <c r="R2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S2" t="s">
         <v>90</v>
@@ -4956,7 +4959,7 @@
         <v>188</v>
       </c>
       <c r="R3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S3" t="s">
         <v>612</v>
@@ -5009,7 +5012,7 @@
         <v>134</v>
       </c>
       <c r="P4" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q4" t="s">
         <v>461</v>
@@ -5074,7 +5077,7 @@
         <v>617</v>
       </c>
       <c r="R5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S5" t="s">
         <v>618</v>
@@ -5133,7 +5136,7 @@
         <v>620</v>
       </c>
       <c r="R6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S6" t="s">
         <v>297</v>
@@ -5251,7 +5254,7 @@
         <v>627</v>
       </c>
       <c r="R8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S8" t="s">
         <v>628</v>
@@ -5304,7 +5307,7 @@
         <v>134</v>
       </c>
       <c r="P9" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q9" t="s">
         <v>414</v>
@@ -5429,7 +5432,7 @@
         <v>45</v>
       </c>
       <c r="Q2" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R2" t="s">
         <v>80</v>
@@ -5470,7 +5473,7 @@
         <v>638</v>
       </c>
       <c r="K3" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L3" t="s">
         <v>44</v>
@@ -5494,7 +5497,7 @@
         <v>154</v>
       </c>
       <c r="S3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.45">
@@ -5632,7 +5635,7 @@
         <v>170</v>
       </c>
       <c r="F6" t="s">
-        <v>533</v>
+        <v>548</v>
       </c>
       <c r="G6" t="s">
         <v>22</v>
@@ -5688,7 +5691,7 @@
         <v>649</v>
       </c>
       <c r="E7" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
@@ -5848,7 +5851,7 @@
         <v>154</v>
       </c>
       <c r="S9" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -6752,10 +6755,10 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>261</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -6773,10 +6776,10 @@
         <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>263</v>
+        <v>228</v>
       </c>
       <c r="K4" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="L4" t="s">
         <v>134</v>
@@ -6794,13 +6797,13 @@
         <v>220</v>
       </c>
       <c r="Q4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R4" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="S4" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.45">
@@ -6814,7 +6817,7 @@
         <v>203</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="E5" t="s">
         <v>176</v>
@@ -6832,10 +6835,10 @@
         <v>52</v>
       </c>
       <c r="J5" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="K5" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="L5" t="s">
         <v>55</v>
@@ -6853,13 +6856,13 @@
         <v>220</v>
       </c>
       <c r="Q5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R5" t="s">
         <v>80</v>
       </c>
       <c r="S5" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.45">
@@ -6873,10 +6876,10 @@
         <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E6" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F6" t="s">
         <v>51</v>
@@ -6888,13 +6891,13 @@
         <v>23</v>
       </c>
       <c r="I6" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="J6" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="K6" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L6" t="s">
         <v>27</v>
@@ -6903,19 +6906,19 @@
         <v>28</v>
       </c>
       <c r="N6" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="O6" t="s">
         <v>134</v>
       </c>
       <c r="P6" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="Q6" t="s">
         <v>159</v>
       </c>
       <c r="R6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S6" t="s">
         <v>100</v>
@@ -6932,10 +6935,10 @@
         <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>240</v>
+        <v>245</v>
       </c>
       <c r="E7" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="F7" t="s">
         <v>21</v>
@@ -6947,10 +6950,10 @@
         <v>23</v>
       </c>
       <c r="I7" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="J7" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="K7" t="s">
         <v>173</v>
@@ -6968,16 +6971,16 @@
         <v>134</v>
       </c>
       <c r="P7" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q7" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="R7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="S7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.45">
@@ -6991,10 +6994,10 @@
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E8" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="F8" t="s">
         <v>21</v>
@@ -7009,10 +7012,10 @@
         <v>52</v>
       </c>
       <c r="J8" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="K8" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="L8" t="s">
         <v>134</v>
@@ -7030,7 +7033,7 @@
         <v>220</v>
       </c>
       <c r="Q8" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="R8" t="s">
         <v>70</v>
@@ -7050,10 +7053,10 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="E9" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -7068,10 +7071,10 @@
         <v>52</v>
       </c>
       <c r="J9" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="K9" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="L9" t="s">
         <v>134</v>
@@ -7089,7 +7092,7 @@
         <v>220</v>
       </c>
       <c r="Q9" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="R9" t="s">
         <v>154</v>
@@ -7109,10 +7112,10 @@
         <v>127</v>
       </c>
       <c r="D10" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="E10" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="F10" t="s">
         <v>21</v>
@@ -7124,10 +7127,10 @@
         <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="J10" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="K10" t="s">
         <v>66</v>
@@ -7145,7 +7148,7 @@
         <v>134</v>
       </c>
       <c r="P10" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q10" t="s">
         <v>32</v>
@@ -7158,9 +7161,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q10">
-    <sortCondition descending="1" ref="E1"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7449,10 +7449,10 @@
         <v>27</v>
       </c>
       <c r="P5" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="Q5" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="R5" t="s">
         <v>80</v>
@@ -7567,7 +7567,7 @@
         <v>134</v>
       </c>
       <c r="P7" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="Q7" t="s">
         <v>296</v>
@@ -7635,7 +7635,7 @@
         <v>80</v>
       </c>
       <c r="S8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.45">
@@ -7851,7 +7851,7 @@
         <v>317</v>
       </c>
       <c r="K2" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="L2" t="s">
         <v>57</v>
@@ -7892,7 +7892,7 @@
         <v>318</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F3" t="s">
         <v>21</v>
@@ -7975,7 +7975,7 @@
         <v>134</v>
       </c>
       <c r="M4" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="N4" t="s">
         <v>106</v>
@@ -8105,7 +8105,7 @@
         <v>45</v>
       </c>
       <c r="Q6" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R6" t="s">
         <v>70</v>
@@ -8205,7 +8205,7 @@
         <v>342</v>
       </c>
       <c r="K8" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
@@ -8466,7 +8466,7 @@
         <v>358</v>
       </c>
       <c r="R3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S3" t="s">
         <v>59</v>
@@ -8525,7 +8525,7 @@
         <v>125</v>
       </c>
       <c r="R4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S4" t="s">
         <v>118</v>
@@ -8569,7 +8569,7 @@
         <v>97</v>
       </c>
       <c r="M5" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="N5" t="s">
         <v>115</v>
@@ -8584,7 +8584,7 @@
         <v>326</v>
       </c>
       <c r="R5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S5" t="s">
         <v>367</v>
@@ -8643,7 +8643,7 @@
         <v>372</v>
       </c>
       <c r="R6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S6" t="s">
         <v>90</v>
@@ -8696,13 +8696,13 @@
         <v>30</v>
       </c>
       <c r="P7" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q7" t="s">
         <v>377</v>
       </c>
       <c r="R7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S7" t="s">
         <v>378</v>
@@ -8740,7 +8740,7 @@
         <v>382</v>
       </c>
       <c r="K8" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="L8" t="s">
         <v>57</v>
@@ -8814,7 +8814,7 @@
         <v>55</v>
       </c>
       <c r="P9" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q9" t="s">
         <v>390</v>
@@ -9234,7 +9234,7 @@
         <v>152</v>
       </c>
       <c r="Q7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="R7" t="s">
         <v>80</v>
@@ -9290,7 +9290,7 @@
         <v>151</v>
       </c>
       <c r="P8" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="Q8" t="s">
         <v>179</v>
@@ -9340,7 +9340,7 @@
         <v>151</v>
       </c>
       <c r="M9" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -9456,7 +9456,7 @@
         <v>427</v>
       </c>
       <c r="K2" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="L2" t="s">
         <v>55</v>
@@ -9574,7 +9574,7 @@
         <v>440</v>
       </c>
       <c r="K4" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="L4" t="s">
         <v>27</v>
@@ -9633,7 +9633,7 @@
         <v>444</v>
       </c>
       <c r="K5" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="L5" t="s">
         <v>134</v>
@@ -9751,7 +9751,7 @@
         <v>454</v>
       </c>
       <c r="K7" t="s">
-        <v>264</v>
+        <v>229</v>
       </c>
       <c r="L7" t="s">
         <v>151</v>
@@ -9851,7 +9851,7 @@
         <v>462</v>
       </c>
       <c r="E9" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="F9" t="s">
         <v>21</v>
@@ -10183,7 +10183,7 @@
         <v>27</v>
       </c>
       <c r="P4" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q4" t="s">
         <v>490</v>
@@ -10248,7 +10248,7 @@
         <v>496</v>
       </c>
       <c r="R5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="S5" t="s">
         <v>160</v>
@@ -10345,7 +10345,7 @@
         <v>504</v>
       </c>
       <c r="K7" t="s">
-        <v>236</v>
+        <v>241</v>
       </c>
       <c r="L7" t="s">
         <v>57</v>
@@ -10537,7 +10537,7 @@
         <v>57</v>
       </c>
       <c r="P10" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="Q10" t="s">
         <v>520</v>

</xml_diff>